<commit_message>
Fixed columnsToKeep and input numbers to null
</commit_message>
<xml_diff>
--- a/src/app/data/Pruebas fisicas.xlsx
+++ b/src/app/data/Pruebas fisicas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FOD_PAGE\fod-pagina\src\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81803147-7598-4FC4-8F0B-CA556AF66A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684EDD6B-EF75-4577-9DC3-1E035F49802F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="-15084" windowWidth="21600" windowHeight="11304" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I56"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>